<commit_message>
22072023 excel file write
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
   <si>
     <t>feature</t>
   </si>
@@ -134,12 +134,25 @@
   </si>
   <si>
     <t>May</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>registration success</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -518,22 +531,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,8 +562,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -566,8 +582,9 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -583,8 +600,9 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -600,8 +618,9 @@
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -617,8 +636,9 @@
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -634,6 +654,7 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -644,15 +665,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -764,20 +787,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.5703125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,8 +818,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -810,8 +838,9 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -827,8 +856,9 @@
       <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -844,8 +874,9 @@
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -861,8 +892,9 @@
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -878,6 +910,7 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="F6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -886,27 +919,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.7109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.5703125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.42578125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.42578125"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.28515625"/>
+    <col min="11" max="11" customWidth="true" width="24.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,8 +971,11 @@
       <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -969,8 +1006,11 @@
       <c r="J2" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -1001,6 +1041,7 @@
       <c r="J3" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="K3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
08102023 list of map to map
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="neworder" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="47">
   <si>
     <t>feature</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>registration success</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>exeflag</t>
+  </si>
+  <si>
+    <t>workflowdescription</t>
   </si>
 </sst>
 </file>
@@ -153,7 +165,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +187,21 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -222,7 +249,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,6 +263,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,133 +568,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.7109375"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.85546875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.7109375"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="1" max="1" customWidth="true" width="11.28515625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125"/>
+    <col min="5" max="5" style="10" width="9.140625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3"/>
+      <c r="H5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -665,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -790,7 +832,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -921,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
bat file added from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="neworder" sheetId="1" r:id="rId1"/>
-    <sheet name="oldorder" sheetId="2" r:id="rId2"/>
-    <sheet name="order" sheetId="3" r:id="rId3"/>
-    <sheet name="register" sheetId="4" r:id="rId4"/>
+    <sheet name="RunBAT" sheetId="5" r:id="rId1"/>
+    <sheet name="neworder" sheetId="1" r:id="rId2"/>
+    <sheet name="oldorder" sheetId="2" r:id="rId3"/>
+    <sheet name="order" sheetId="3" r:id="rId4"/>
+    <sheet name="register" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -161,7 +162,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +184,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,9 +554,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -674,8 +701,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -772,8 +800,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -858,8 +887,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>